<commit_message>
updated changelog and folders
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -28,29 +28,75 @@
     <t xml:space="preserve">Finish Time</t>
   </si>
   <si>
-    <t xml:space="preserve">Hours Logged</t>
+    <t xml:space="preserve">Minutes Logged</t>
   </si>
   <si>
     <t xml:space="preserve">1:00PM 6-15-2017</t>
   </si>
   <si>
-    <t xml:space="preserve">2:53PM 6-15-2017</t>
+    <t xml:space="preserve">2:30PM 6-15-2017</t>
   </si>
   <si>
     <t xml:space="preserve">7:11PM 10-26-2017</t>
   </si>
   <si>
+    <t xml:space="preserve">9:30AM 10-27-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:40PM 10-26-2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">12:12AM 10-27-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:40PM 10-28-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:39PM 10-28-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:00PM 10-28-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:13PM 10-28-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:15PM 11-22-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:15AM 11-23-2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:28PM 11-23-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01:19PM 11-23-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:10PM 11-23-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:06PM 11-23-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:18AM 11-24-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:59PM 11-24-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Project Hours:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -72,50 +118,73 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
+      <b val="true"/>
+      <sz val="24"/>
       <color rgb="FF000000"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="FreeSans"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="FreeSans"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -217,25 +286,65 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,10 +441,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -344,7 +453,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -367,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,13 +487,93 @@
         <v>6</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>4</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="C4" s="0" t="n">
-        <f aca="false">SUM(C2:C3)</f>
-        <v>5.5</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <f aca="false">SUM(C2:C16)/60</f>
+        <v>24.0166666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
overlap detection binary utilized by php script : ). Works as planned.
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t xml:space="preserve">7:46PM 11-24-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:36AM 12-28-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:38PM 12-28-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:54PM 12-12-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:42PM 12-28-2017</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -102,7 +114,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -124,16 +136,139 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -141,8 +276,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -166,6 +316,54 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -181,14 +379,90 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -199,13 +473,13 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.14"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="18.06"/>
@@ -334,13 +608,35 @@
         <v>176</v>
       </c>
     </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>228</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">SUM(C2:C16)/60</f>
-        <v>26.95</v>
+        <v>31.7833333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
not sure why the changes from the last commit didnt save...
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t xml:space="preserve">5:42PM 12-28-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:34PM 12-29-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5:04PM 12-29-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:01PM 12-30-2017</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -119,7 +128,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,28 +150,24 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -171,28 +175,24 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -200,7 +200,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -208,14 +207,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -474,7 +471,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -630,13 +627,29 @@
         <v>228</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">SUM(C2:C16)/60</f>
-        <v>31.7833333333333</v>
+        <v>33.2833333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrote php shape class clipping algorithm to fully utilize overlap code in php
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t xml:space="preserve">6:01PM 12-30-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:15PM 12-30-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:00AM 12-31-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:52PM 12-31-2017</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -128,6 +137,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -150,24 +160,28 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -175,24 +189,28 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -200,6 +218,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -207,12 +226,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -471,7 +492,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -642,14 +663,31 @@
       <c r="A15" s="0" t="s">
         <v>29</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>172</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">SUM(C2:C16)/60</f>
-        <v>33.2833333333333</v>
+        <v>37.3833333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Began file IO and garden inheritence
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">12:38PM 12-28-2017</t>
   </si>
   <si>
-    <t xml:space="preserve">1:54PM 12-12-2017</t>
+    <t xml:space="preserve">1:54PM 12-28-2017</t>
   </si>
   <si>
     <t xml:space="preserve">5:42PM 12-28-2017</t>
@@ -119,6 +119,24 @@
   </si>
   <si>
     <t xml:space="preserve">12:52PM 12-31-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:04 PM 12-31-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:47 PM 12-31-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:23 PM 12-31-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:19 PM 12-31-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:32PM 12-31-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:32PM 12-31-2017</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -489,10 +507,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -682,12 +700,45 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="B17" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="C17" s="0" t="n">
-        <f aca="false">SUM(C2:C16)/60</f>
-        <v>37.3833333333333</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <f aca="false">SUM(C2:C20)/60</f>
+        <v>43.0333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on garden file I/O
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -142,7 +142,13 @@
     <t xml:space="preserve">11:54PM 1-17-2018</t>
   </si>
   <si>
-    <t xml:space="preserve">1:14 1-17-2018</t>
+    <t xml:space="preserve">1:14AM 1-17-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:33PM 1-19-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:06PM 1-19-2018</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -513,10 +519,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -753,9 +759,20 @@
       <c r="A21" s="0" t="s">
         <v>41</v>
       </c>
+      <c r="B21" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="C21" s="0" t="n">
-        <f aca="false">SUM(C2:C20)/60</f>
-        <v>44.3666666666667</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <f aca="false">SUM(C2:C28)/60</f>
+        <v>46.9166666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
designed .garden file in plans folder and finished IO
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t xml:space="preserve">9:06PM 1-19-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:58PM 1-19-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:55PM 1-19-2018</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -522,7 +528,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -766,13 +772,24 @@
         <v>153</v>
       </c>
     </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">SUM(C2:C28)/60</f>
-        <v>46.9166666666667</v>
+        <v>47.8666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished structure.garden in plans folder to give an example of the save file.
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t xml:space="preserve">11:55PM 1-19-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:08PM 1-20-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:21PM 1-20-2018</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -528,7 +534,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -783,13 +789,24 @@
         <v>57</v>
       </c>
     </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>133</v>
+      </c>
+    </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">SUM(C2:C28)/60</f>
-        <v>47.8666666666667</v>
+        <v>50.0833333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried using the usda plant database api https://plantsdb.xyz/search (see home.php in this commit), yet common name search failed with names like "Green Beans" or "Bell Peppers" due to common misnomers. Implemented more practical approach of simple_html_dom and google image parse, using the common name that the user types to fetch an image and displayed the typed name verbatim
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t xml:space="preserve">2:21PM 1-20-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:32PM 1-20-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:23PM 1-20-2018</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -534,7 +540,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -800,13 +806,24 @@
         <v>133</v>
       </c>
     </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>171</v>
+      </c>
+    </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">SUM(C2:C28)/60</f>
-        <v>50.0833333333333</v>
+        <v>52.9333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
not pretty, but tons of progress
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t xml:space="preserve">7:23PM 1-20-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:30PM 1-20-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:45PM 1-20-2018</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -539,8 +545,8 @@
   </sheetPr>
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -817,13 +823,24 @@
         <v>171</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>75</v>
+      </c>
+    </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">SUM(C2:C28)/60</f>
-        <v>52.9333333333333</v>
+        <v>54.1833333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fileIO load feature to accept the new .garden format entirely
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -173,6 +173,30 @@
   </si>
   <si>
     <t xml:space="preserve">10:45PM 1-20-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:41AM 1-21-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:32AM 1-21-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:07AM 1-21-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:47AM 1-21-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2:07PM 1-21-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:04PM 1-21-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:08PM 1-21-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8:00PM 1-21-2018</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -543,10 +567,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -834,13 +858,57 @@
         <v>75</v>
       </c>
     </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="C29" s="0" t="n">
-        <f aca="false">SUM(C2:C28)/60</f>
-        <v>54.1833333333333</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <f aca="false">SUM(C2:C39)/60</f>
+        <v>59.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
drawing shapes in js, created the algorithm to draw the garden and save it. Experimented with click handlers in th konva library
</commit_message>
<xml_diff>
--- a/Volunteer Hours.xlsx
+++ b/Volunteer Hours.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t xml:space="preserve">Start Time</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t xml:space="preserve">8:00PM 1-21-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:31AM 2-25-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:17PM 2-25-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4:43PM 2-25-2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9:11PM 2-25-2018</t>
   </si>
   <si>
     <t xml:space="preserve">Total Project Hours:</t>
@@ -570,7 +582,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -902,13 +914,35 @@
         <v>52</v>
       </c>
     </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>268</v>
+      </c>
+    </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C40" s="0" t="n">
         <f aca="false">SUM(C2:C39)/60</f>
-        <v>59.45</v>
+        <v>65.6833333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>